<commit_message>
updated tt file for wednesday
</commit_message>
<xml_diff>
--- a/timetable2.xlsx
+++ b/timetable2.xlsx
@@ -369,6 +369,9 @@
     <t xml:space="preserve">TE5(EC411)-229/VG</t>
   </si>
   <si>
+    <t xml:space="preserve">WED</t>
+  </si>
+  <si>
     <t xml:space="preserve">LE1E2E3E4E5E6E7E8 (16B1NHS431)-
 118A/PRV</t>
   </si>
@@ -410,9 +413,6 @@
   </si>
   <si>
     <t xml:space="preserve">PE6(EC472)-133/YOGESH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WED</t>
   </si>
   <si>
     <t xml:space="preserve">PE6(EC471)-134/HEMANT</t>
@@ -1087,7 +1087,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1128,7 +1128,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1136,12 +1136,12 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1150,6 +1150,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="90" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1183,17 +1187,17 @@
   </sheetPr>
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A23" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I28" activeCellId="0" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="15.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.51"/>
@@ -1738,7 +1742,9 @@
       <c r="J25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="12" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10"/>
+      <c r="A26" s="10" t="s">
+        <v>115</v>
+      </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1756,10 +1762,10 @@
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="8" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F27" s="11" t="s">
         <v>72</v>
@@ -1779,68 +1785,66 @@
         <v>65</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="F28" s="11"/>
       <c r="G28" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H28" s="6"/>
       <c r="I28" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="J28" s="6"/>
     </row>
     <row r="29" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="10"/>
       <c r="B29" s="6" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="6" t="s">
         <v>70</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H29" s="6"/>
       <c r="I29" s="2"/>
       <c r="J29" s="6" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="10"/>
       <c r="B30" s="6" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C30" s="6"/>
       <c r="D30" s="6" t="s">
         <v>77</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F30" s="9"/>
       <c r="G30" s="6" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="J30" s="6"/>
     </row>
     <row r="31" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="12" t="s">
-        <v>129</v>
-      </c>
+      <c r="A31" s="10"/>
       <c r="B31" s="6" t="s">
         <v>130</v>
       </c>
@@ -1866,7 +1870,7 @@
       <c r="J31" s="6"/>
     </row>
     <row r="32" customFormat="false" ht="17.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="12"/>
+      <c r="A32" s="10"/>
       <c r="B32" s="6" t="s">
         <v>135</v>
       </c>
@@ -1890,7 +1894,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="12"/>
+      <c r="A33" s="10"/>
       <c r="B33" s="6" t="s">
         <v>45</v>
       </c>
@@ -1909,12 +1913,12 @@
       <c r="I33" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="J33" s="13" t="s">
+      <c r="J33" s="12" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="23.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="12"/>
+      <c r="A34" s="10"/>
       <c r="B34" s="6" t="s">
         <v>143</v>
       </c>
@@ -1936,7 +1940,7 @@
       <c r="J34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="12"/>
+      <c r="A35" s="10"/>
       <c r="B35" s="6" t="s">
         <v>147</v>
       </c>
@@ -1958,7 +1962,7 @@
       <c r="J35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="12"/>
+      <c r="A36" s="10"/>
       <c r="B36" s="6" t="s">
         <v>152</v>
       </c>
@@ -1978,7 +1982,7 @@
       <c r="J36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="12"/>
+      <c r="A37" s="10"/>
       <c r="B37" s="2"/>
       <c r="C37" s="6" t="s">
         <v>156</v>
@@ -1994,7 +1998,7 @@
       <c r="J37" s="2"/>
     </row>
     <row r="38" customFormat="false" ht="11.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="12"/>
+      <c r="A38" s="13"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
@@ -2027,7 +2031,7 @@
       <c r="A40" s="5"/>
       <c r="B40" s="2"/>
       <c r="C40" s="6" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="D40" s="6"/>
       <c r="E40" s="2"/>
@@ -2394,7 +2398,7 @@
       </c>
       <c r="E59" s="2"/>
       <c r="F59" s="9" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
@@ -2433,7 +2437,7 @@
       </c>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
-      <c r="F61" s="10"/>
+      <c r="F61" s="16"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -2447,7 +2451,7 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
-      <c r="F62" s="10"/>
+      <c r="F62" s="16"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -2459,19 +2463,19 @@
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
-      <c r="F63" s="10"/>
+      <c r="F63" s="16"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
       <c r="J63" s="2"/>
     </row>
     <row r="64" customFormat="false" ht="11.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="16"/>
+      <c r="A64" s="17"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
-      <c r="F64" s="16"/>
+      <c r="F64" s="17"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -2621,7 +2625,7 @@
       <c r="G73" s="4"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
-      <c r="J73" s="17"/>
+      <c r="J73" s="18"/>
     </row>
     <row r="74" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="2"/>
@@ -2823,10 +2827,10 @@
       <c r="C82" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="D82" s="18" t="n">
+      <c r="D82" s="19" t="n">
         <v>142</v>
       </c>
-      <c r="E82" s="18"/>
+      <c r="E82" s="19"/>
       <c r="F82" s="9" t="s">
         <v>287</v>
       </c>
@@ -2954,7 +2958,7 @@
       <c r="J87" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="118">
+  <mergeCells count="117">
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A3:A13"/>
     <mergeCell ref="D3:E3"/>
@@ -2987,7 +2991,7 @@
     <mergeCell ref="F21:F22"/>
     <mergeCell ref="I21:J21"/>
     <mergeCell ref="F23:F25"/>
-    <mergeCell ref="A26:A30"/>
+    <mergeCell ref="A26:A37"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="H27:I27"/>
@@ -3000,7 +3004,6 @@
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="G30:H30"/>
     <mergeCell ref="I30:J30"/>
-    <mergeCell ref="A31:A38"/>
     <mergeCell ref="B31:C31"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="I31:J31"/>

</xml_diff>